<commit_message>
Este es mi primer commit
</commit_message>
<xml_diff>
--- a/archivo1.xlsx
+++ b/archivo1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t xml:space="preserve">archivo 2 </t>
   </si>
@@ -37,6 +37,39 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>Nombres</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
 </sst>
 </file>
@@ -78,7 +111,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -354,20 +398,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -384,535 +428,603 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f ca="1">RAND()</f>
-        <v>0.86797910088208496</v>
+        <v>0.7507416695502459</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:E3" ca="1" si="0">RAND()</f>
-        <v>0.71298152466447651</v>
+        <v>0.29041894685079117</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21142124357929881</v>
+        <v>0.73010367707757462</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29262599728131622</v>
+        <v>0.30677804433690414</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9214772702378524E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.77198972752864481</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:E26" ca="1" si="1">RAND()</f>
-        <v>8.9556422737540609E-2</v>
+        <v>0.38865815773654966</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.13651589500074213</v>
+        <v>0.28796807853735207</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39772281186185976</v>
+        <v>0.53236006558209348</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81911161018763401</v>
+        <v>3.4921852435590983E-3</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36181002585800792</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.53419147468840333</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61903183987513022</v>
+        <v>0.71236191141344385</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.70026089233725208</v>
+        <v>0.86425314776575946</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8147135592078838E-2</v>
+        <v>0.35175027018528893</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94309089954971526</v>
+        <v>0.24708462648208274</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97429137998358084</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.23612516750933554</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.40670875606631895</v>
+        <v>3.03085456977914E-2</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26903092969590514</v>
+        <v>0.61333904655133975</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60735317567081692</v>
+        <v>0.13952667702132449</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23356133138675184</v>
+        <v>0.92883059793384803</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59375803637601687</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5.8323862633949841E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20147760375198609</v>
+        <v>0.58957601593597075</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73388606839275206</v>
+        <v>0.53103785873741283</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.65320237467672648</v>
+        <v>0.36015422721848189</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23782449137153283</v>
+        <v>0.18674427636730884</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47230717443450243</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2.1820523113623813E-2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68912313858837659</v>
+        <v>0.28249132896343843</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9737223720446232</v>
+        <v>0.68664381118325146</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63749106708982883</v>
+        <v>9.5789399624044536E-2</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59795647435861787</v>
+        <v>0.42988464278498562</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9876061490675565E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.44598085667364673</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>3.7339838681427984E-2</v>
+        <v>0.52150714845655688</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.91557977113211786</v>
+        <v>0.85861138989142316</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20039642778856026</v>
+        <v>0.20776718302581798</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.82524988488779072</v>
+        <v>0.32455962114557313</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4190830205645875E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.11291978422981219</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87628244768624952</v>
+        <v>0.45679945894857843</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39636860220803183</v>
+        <v>0.4352853995397411</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.78076415199455951</v>
+        <v>0.17658366481806753</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42327717910912999</v>
+        <v>0.34772685079053189</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.76509953518723972</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.85423646377644824</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46789188330131715</v>
+        <v>0.53931335449457007</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46312114577338015</v>
+        <v>0.63943055936468807</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16476994511090826</v>
+        <v>0.64392335273666657</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.3372047766741898</v>
+        <v>0.30983091835316001</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.40666936237572138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.4852250017026114</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11191355727295471</v>
+        <v>0.7267763628137387</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0614390678304901E-2</v>
+        <v>0.31183340097432577</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58446894551232864</v>
+        <v>0.28958735866158225</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56914650795510113</v>
+        <v>0.49559189100078904</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17411469391107559</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.46453343718449147</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4962987515720356E-2</v>
+        <v>0.99645814749772565</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8872204132635193</v>
+        <v>0.22738380055093821</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47525834932810629</v>
+        <v>0.41600556494305818</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22095569636525059</v>
+        <v>0.7522968465805836</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.55348510747681878</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.44000509779871499</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58917334828291856</v>
+        <v>0.98811648260688012</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46830839408465608</v>
+        <v>0.92998615111059069</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16785040131725404</v>
+        <v>0.2229735299756096</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26986902129479551</v>
+        <v>0.14511020122951312</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46899365360707723</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.4142280643362326</v>
+      </c>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89723807913757014</v>
+        <v>0.25296335147908477</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25257938639123478</v>
+        <v>0.56786613216963611</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69158840014981027</v>
+        <v>0.89984309843610011</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88524696030443106</v>
+        <v>0.73603195369835284</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41570555266661413</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.10026648307115693</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27867449418596679</v>
+        <v>0.31091894318440116</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87782912882732989</v>
+        <v>0.10232332282198231</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1821026842910427</v>
+        <v>0.52152646016724447</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.59741117181963999</v>
+        <v>0.22840252018309459</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7372415300620635</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.2664346923251959</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94683185957198313</v>
+        <v>0.63931235566786115</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60759862831008893</v>
+        <v>0.28998946183019436</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35508824675969153</v>
+        <v>2.9277683146474831E-2</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53408502266343949</v>
+        <v>0.6436053743278537</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.74270406152100232</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.43534608255532903</v>
+      </c>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.9937042355739677</v>
+        <v>0.67214199108631878</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46076235841325386</v>
+        <v>0.60013826102184709</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34741099132060915</v>
+        <v>0.20062728536902086</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2196920203552155E-3</v>
+        <v>0.92808088602738292</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17024802226782287</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.84298280302687056</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61611473553905949</v>
+        <v>0.10695834947532046</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>9.7785750077879707E-2</v>
+        <v>0.94952513960955043</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.69907677953279901</v>
+        <v>0.24828012583121084</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63814479654930167</v>
+        <v>0.75013085778797717</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.88980462120314507</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.36757250084517501</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47904615525113126</v>
+        <v>7.4779543668726967E-2</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.5671772991101226</v>
+        <v>0.4772256779608619</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87431991560872047</v>
+        <v>0.64867557270454357</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.97463113519058164</v>
+        <v>0.14500734856484532</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.13027090665358154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.38576075109133412</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46538754954637063</v>
+        <v>1.8212167753970387E-2</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.39458696017546158</v>
+        <v>0.41620097907835429</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6290740314207026E-2</v>
+        <v>0.37013689134609218</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>5.5987603994026247E-2</v>
+        <v>0.12701519157380259</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63300367539915403</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.44788867898247764</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1906402905826895</v>
+        <v>0.35468519966668399</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80259348826031496</v>
+        <v>0.21308864150825602</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89018206167946001</v>
+        <v>0.1848928656431259</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24011630984185584</v>
+        <v>0.49098661738544436</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60129864658440857</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.12838656552002403</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28417157624460598</v>
+        <v>6.891674879850751E-2</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54148049737470993</v>
+        <v>0.66588210069957054</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>3.0192068593913657E-2</v>
+        <v>0.27415620021257947</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21464559622151269</v>
+        <v>0.71424543890640435</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5127841799222228E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.8133770698941496</v>
+      </c>
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.87363027406831395</v>
+        <v>0.75541791682182813</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11450748827284707</v>
+        <v>0.77640082018633194</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99601772152055845</v>
+        <v>0.18208890420803348</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34694799540747001</v>
+        <v>0.32180615368168686</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16249833021428561</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.11576853772193585</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0331896208312132E-3</v>
+        <v>0.99942110866391165</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.19574038401678329</v>
+        <v>0.92269212306394499</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.57231995056951845</v>
+        <v>0.42858360801227935</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63875275268531839</v>
+        <v>0.36342623821924136</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53736461837411742</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.16455164411948275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94024918756865894</v>
+        <v>0.73266085748308796</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7813398620876798</v>
+        <v>0.13477942715446134</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10925364358759049</v>
+        <v>0.10282498535655349</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.80606333408613939</v>
+        <v>0.34936057614331972</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18943240544049156</v>
+        <v>0.34613773173670426</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G4:G23">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="a">
+      <formula>NOT(ISERROR(SEARCH("a",G4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
primer commit de la rama uno, tercer commit en general
</commit_message>
<xml_diff>
--- a/archivo1.xlsx
+++ b/archivo1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t xml:space="preserve">archivo 2 </t>
   </si>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="G19" sqref="G19:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,23 +431,23 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f ca="1">RAND()</f>
-        <v>0.7507416695502459</v>
+        <v>9.0097444856769848E-2</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:E3" ca="1" si="0">RAND()</f>
-        <v>0.29041894685079117</v>
+        <v>0.78622200261172737</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73010367707757462</v>
+        <v>0.101367330268053</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30677804433690414</v>
+        <v>0.23699189199307513</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77198972752864481</v>
+        <v>0.22186007627989879</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -456,23 +456,23 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:E26" ca="1" si="1">RAND()</f>
-        <v>0.38865815773654966</v>
+        <v>0.90275469405287267</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28796807853735207</v>
+        <v>0.72262408076432594</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53236006558209348</v>
+        <v>0.10253027037766993</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4921852435590983E-3</v>
+        <v>0.89253172490880395</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53419147468840333</v>
+        <v>0.43619702355349266</v>
       </c>
       <c r="G4" t="s">
         <v>7</v>
@@ -481,23 +481,23 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71236191141344385</v>
+        <v>0.62931324521015408</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.86425314776575946</v>
+        <v>0.49596439237111478</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35175027018528893</v>
+        <v>7.383746474197328E-2</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24708462648208274</v>
+        <v>0.26996273755873912</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.23612516750933554</v>
+        <v>0.87773942208419675</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -506,23 +506,23 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>3.03085456977914E-2</v>
+        <v>0.93541106878187674</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.61333904655133975</v>
+        <v>0.79627200926494868</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.13952667702132449</v>
+        <v>0.3223230929165678</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92883059793384803</v>
+        <v>0.84187903581294443</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8323862633949841E-2</v>
+        <v>0.50753878530607388</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -531,23 +531,23 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.58957601593597075</v>
+        <v>7.8511182305021521E-2</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53103785873741283</v>
+        <v>0.47388614982910149</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36015422721848189</v>
+        <v>0.73641248774395063</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18674427636730884</v>
+        <v>5.6553971937768899E-2</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1820523113623813E-2</v>
+        <v>0.94711416822242533</v>
       </c>
       <c r="G7" t="s">
         <v>10</v>
@@ -556,23 +556,23 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28249132896343843</v>
+        <v>6.2944808921425954E-2</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68664381118325146</v>
+        <v>0.327888563122262</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5789399624044536E-2</v>
+        <v>0.12538577925943617</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42988464278498562</v>
+        <v>0.65378923710094949</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44598085667364673</v>
+        <v>0.72642413927274274</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -581,23 +581,23 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52150714845655688</v>
+        <v>0.99637899884590031</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85861138989142316</v>
+        <v>0.74630558334222474</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20776718302581798</v>
+        <v>0.93468988515363938</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32455962114557313</v>
+        <v>0.10223974646556044</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11291978422981219</v>
+        <v>0.79635990459654227</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
@@ -606,23 +606,23 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.45679945894857843</v>
+        <v>0.82848406156656218</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4352853995397411</v>
+        <v>0.55962092042081402</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17658366481806753</v>
+        <v>0.63772652826652154</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34772685079053189</v>
+        <v>0.14321789461242396</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.85423646377644824</v>
+        <v>0.20971423589866134</v>
       </c>
       <c r="G10" t="s">
         <v>13</v>
@@ -631,23 +631,23 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.53931335449457007</v>
+        <v>0.51163666936291052</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63943055936468807</v>
+        <v>0.87535400842045286</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64392335273666657</v>
+        <v>0.90233430713245322</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.30983091835316001</v>
+        <v>0.70948425761478739</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4852250017026114</v>
+        <v>0.66848386069464638</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
@@ -656,23 +656,23 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7267763628137387</v>
+        <v>0.90811982324903395</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31183340097432577</v>
+        <v>0.29646941391844428</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28958735866158225</v>
+        <v>0.42109087130977629</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49559189100078904</v>
+        <v>0.56161581537831351</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46453343718449147</v>
+        <v>0.24311798603269263</v>
       </c>
       <c r="G12" t="s">
         <v>15</v>
@@ -681,23 +681,23 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99645814749772565</v>
+        <v>0.53669581540495936</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22738380055093821</v>
+        <v>0.72950679459058287</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41600556494305818</v>
+        <v>6.4197299080647197E-2</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.7522968465805836</v>
+        <v>0.35270953634724667</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44000509779871499</v>
+        <v>0.14908086814626886</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
@@ -706,23 +706,23 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.98811648260688012</v>
+        <v>0.80542211872206537</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92998615111059069</v>
+        <v>0.38321400307511844</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2229735299756096</v>
+        <v>0.83770310325236685</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.14511020122951312</v>
+        <v>0.12524570343630881</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4142280643362326</v>
+        <v>0.54837272048425756</v>
       </c>
       <c r="G14" t="s">
         <v>7</v>
@@ -731,23 +731,23 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.25296335147908477</v>
+        <v>0.46863823265177884</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.56786613216963611</v>
+        <v>0.41741822871584222</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.89984309843610011</v>
+        <v>0.82219548837125822</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73603195369835284</v>
+        <v>0.17225822309338934</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10026648307115693</v>
+        <v>0.70744990809452257</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
@@ -756,271 +756,289 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.31091894318440116</v>
+        <v>0.12132429421645119</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10232332282198231</v>
+        <v>0.11079319089921935</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.52152646016724447</v>
+        <v>0.67887298212784386</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.22840252018309459</v>
+        <v>0.75886503423026985</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2664346923251959</v>
+        <v>0.88286952662083162</v>
       </c>
       <c r="G16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.63931235566786115</v>
+        <v>0.36058168946141622</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28998946183019436</v>
+        <v>0.69224399039846363</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9277683146474831E-2</v>
+        <v>0.85187288317466803</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.6436053743278537</v>
+        <v>0.11712856149266637</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>0.43534608255532903</v>
+        <v>0.56323110228138129</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67214199108631878</v>
+        <v>7.5092284016778588E-2</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.60013826102184709</v>
+        <v>0.81979572237500264</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20062728536902086</v>
+        <v>0.94656167588085871</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92808088602738292</v>
+        <v>0.37848979662963944</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.84298280302687056</v>
+        <v>3.3006216263946286E-2</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10695834947532046</v>
+        <v>0.26751743580178478</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.94952513960955043</v>
+        <v>0.87588148281104883</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.24828012583121084</v>
+        <v>0.1638801095599679</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.75013085778797717</v>
+        <v>0.87372982707759861</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36757250084517501</v>
+        <v>0.41751965382579637</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" t="s">
+        <v>12</v>
+      </c>
+      <c r="M19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>7.4779543668726967E-2</v>
+        <v>0.44345408473430015</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.4772256779608619</v>
+        <v>0.94579756654303315</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.64867557270454357</v>
+        <v>0.97207919744345828</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.14500734856484532</v>
+        <v>0.80042305939512226</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38576075109133412</v>
+        <v>0.28346088793393431</v>
       </c>
       <c r="G20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8212167753970387E-2</v>
+        <v>0.18366991158116919</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.41620097907835429</v>
+        <v>0.23014484999669704</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.37013689134609218</v>
+        <v>0.2221106889896507</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12701519157380259</v>
+        <v>0.37085849039988994</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44788867898247764</v>
+        <v>0.82216090957268695</v>
       </c>
       <c r="G21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.35468519966668399</v>
+        <v>0.85611251770566843</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21308864150825602</v>
+        <v>0.36840770714529514</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.1848928656431259</v>
+        <v>0.25022445360192547</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.49098661738544436</v>
+        <v>0.46412308502474464</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.12838656552002403</v>
+        <v>0.16155967172575636</v>
       </c>
       <c r="G22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>6.891674879850751E-2</v>
+        <v>0.18725645842628547</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.66588210069957054</v>
+        <v>0.84930148811363093</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.27415620021257947</v>
+        <v>3.8943514601316176E-3</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.71424543890640435</v>
+        <v>0.12886557753733974</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8133770698941496</v>
+        <v>0.25522187220148418</v>
       </c>
       <c r="G23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.75541791682182813</v>
+        <v>0.63244913912450662</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.77640082018633194</v>
+        <v>0.22743771467651497</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.18208890420803348</v>
+        <v>0.81680026096746061</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.32180615368168686</v>
+        <v>0.5678724493811409</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.11576853772193585</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.71722152815692708</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99942110866391165</v>
+        <v>0.9843337566703283</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.92269212306394499</v>
+        <v>0.83991686887098349</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42858360801227935</v>
+        <v>0.30301382018417644</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.36342623821924136</v>
+        <v>0.88296811021177346</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.16455164411948275</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.4889921865532396E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.73266085748308796</v>
+        <v>0.75070757119018949</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.13477942715446134</v>
+        <v>0.36454349987114743</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10282498535655349</v>
+        <v>0.67461446076931331</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34936057614331972</v>
+        <v>0.78763967941615975</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34613773173670426</v>
+        <v>0.71662502887229607</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G4:G23">
+  <conditionalFormatting sqref="G4:G23 H19:M19">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="a">
       <formula>NOT(ISERROR(SEARCH("a",G4)))</formula>
     </cfRule>

</xml_diff>